<commit_message>
Finished schematic. Started working on PCB layout
</commit_message>
<xml_diff>
--- a/Components/BOM.xlsx
+++ b/Components/BOM.xlsx
@@ -5,22 +5,33 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Function-Generator\PCB Parts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Function-Generator\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7375E909-D59B-4429-B4C9-597DE4C0B8C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B429768-53FD-4105-B3B7-74FFE801DD46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Index</t>
   </si>
@@ -290,6 +301,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Digikey Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>Total Price</t>
   </si>
 </sst>
 </file>
@@ -646,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -665,7 +679,7 @@
     <col min="10" max="10" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,8 +710,11 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -725,8 +742,12 @@
       <c r="J2" s="3">
         <v>1.08</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <f>I2*B2</f>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -754,8 +775,12 @@
       <c r="J3" s="3">
         <v>1.08</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <f t="shared" ref="K3:K28" si="0">I3*B3</f>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -783,8 +808,12 @@
       <c r="J4" s="3">
         <v>1.49</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -812,8 +841,12 @@
       <c r="J5" s="3">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -841,8 +874,12 @@
       <c r="J6" s="3">
         <v>1.04</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="2">
         <v>7</v>
       </c>
@@ -870,8 +907,12 @@
       <c r="J7" s="3">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="2">
         <v>8</v>
       </c>
@@ -899,8 +940,12 @@
       <c r="J8" s="3">
         <v>1.1599999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>1.1600000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="2">
         <v>9</v>
       </c>
@@ -928,8 +973,12 @@
       <c r="J9" s="3">
         <v>0.79</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="2">
         <v>10</v>
       </c>
@@ -957,8 +1006,12 @@
       <c r="J10" s="3">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>0.41000000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="2">
         <v>11</v>
       </c>
@@ -986,8 +1039,12 @@
       <c r="J11" s="3">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="2">
         <v>12</v>
       </c>
@@ -1015,8 +1072,12 @@
       <c r="J12" s="3">
         <v>1.73</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="2">
         <v>13</v>
       </c>
@@ -1044,8 +1105,12 @@
       <c r="J13" s="3">
         <v>10.16</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>10.16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="2">
         <v>14</v>
       </c>
@@ -1073,8 +1138,12 @@
       <c r="J14" s="3">
         <v>1.1100000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="2">
         <v>18</v>
       </c>
@@ -1102,8 +1171,12 @@
       <c r="J15" s="3">
         <v>6.15</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>6.1499999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="2">
         <v>19</v>
       </c>
@@ -1131,8 +1204,12 @@
       <c r="J16" s="3">
         <v>2.66</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="2">
         <v>20</v>
       </c>
@@ -1160,8 +1237,12 @@
       <c r="J17" s="3">
         <v>1.53</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="2">
         <v>21</v>
       </c>
@@ -1189,8 +1270,12 @@
       <c r="J18" s="3">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="2">
         <v>22</v>
       </c>
@@ -1218,8 +1303,12 @@
       <c r="J19" s="3">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>0.9900000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="2">
         <v>23</v>
       </c>
@@ -1247,8 +1336,12 @@
       <c r="J20" s="3">
         <v>1.0900000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="2">
         <v>24</v>
       </c>
@@ -1276,8 +1369,12 @@
       <c r="J21" s="3">
         <v>1.0900000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="2">
         <v>25</v>
       </c>
@@ -1305,8 +1402,12 @@
       <c r="J22" s="3">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>0.8899999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="2">
         <v>26</v>
       </c>
@@ -1334,8 +1435,12 @@
       <c r="J23" s="3">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>0.70000000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="2">
         <v>30</v>
       </c>
@@ -1363,8 +1468,12 @@
       <c r="J24" s="3">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="2">
         <v>32</v>
       </c>
@@ -1392,8 +1501,12 @@
       <c r="J25" s="3">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="2">
         <v>33</v>
       </c>
@@ -1421,8 +1534,12 @@
       <c r="J26" s="3">
         <v>4.9400000000000004</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>4.9400000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="2">
         <v>34</v>
       </c>
@@ -1450,8 +1567,12 @@
       <c r="J27" s="3">
         <v>4.16</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="2">
         <v>35</v>
       </c>
@@ -1478,6 +1599,16 @@
       </c>
       <c r="J28" s="3">
         <v>2.36</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="K29">
+        <f>SUM(K2:K28)</f>
+        <v>64.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>